<commit_message>
add h_degree calculation code and save results
</commit_message>
<xml_diff>
--- a/statistic_info_hete_datasets.xlsx
+++ b/statistic_info_hete_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiqiang.zhong\PhD_UL\PhD_Project\coarsening-disassortative-graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ECE0D6-590D-4A40-A048-6F257FACBC85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4265DB-D8EB-4737-86E0-03DDFB0387AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{3BD7E531-4CDA-40A9-9528-C404C0AADB91}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -121,13 +121,16 @@
   </si>
   <si>
     <t>OOM</t>
+  </si>
+  <si>
+    <t>h_degree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +168,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,23 +195,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,81 +536,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40115779-E315-4549-B12D-99D51145727F}">
-  <dimension ref="B9:M30"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B9:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
-    <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1"/>
-    <col min="17" max="18" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="18" max="19" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="J9" s="5" t="s">
+    <row r="9" spans="2:14" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="4" t="s">
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="6"/>
+      <c r="M10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="M11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="N11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -617,11 +640,17 @@
       <c r="I12">
         <v>0.622</v>
       </c>
-      <c r="K12">
+      <c r="J12" s="9">
+        <v>0.107</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
         <v>0.2762</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -646,11 +675,17 @@
       <c r="I13">
         <v>0.21199999999999999</v>
       </c>
-      <c r="K13">
+      <c r="J13" s="9">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
         <v>6.9800000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,11 +710,17 @@
       <c r="I14">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K14">
+      <c r="J14" s="9">
+        <v>-0.3463</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
         <v>0.10009999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -704,11 +745,17 @@
       <c r="I15">
         <v>0.17199999999999999</v>
       </c>
-      <c r="K15">
+      <c r="J15" s="9">
+        <v>-0.2883</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
         <v>9.7199999999999995E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -733,11 +780,17 @@
       <c r="I16">
         <v>0.246</v>
       </c>
-      <c r="K16">
+      <c r="J16" s="9">
+        <v>-5.2400000000000002E-2</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9">
         <v>9.8400000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -762,11 +815,17 @@
       <c r="I17">
         <v>0.221</v>
       </c>
-      <c r="K17">
+      <c r="J17" s="9">
+        <v>8.2100000000000006E-2</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9">
         <v>1.1299999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -791,11 +850,17 @@
       <c r="I18">
         <v>0.29799999999999999</v>
       </c>
-      <c r="K18">
+      <c r="J18" s="9">
+        <v>-0.1181</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9">
         <v>0.16919999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
@@ -820,11 +885,17 @@
       <c r="I19">
         <v>0.159</v>
       </c>
-      <c r="K19">
+      <c r="J19" s="9">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
@@ -849,11 +920,17 @@
       <c r="I20">
         <v>0.53</v>
       </c>
-      <c r="K20" t="s">
+      <c r="J20" s="9">
+        <v>0.1399</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>15</v>
       </c>
@@ -878,11 +955,17 @@
       <c r="I21">
         <v>0.64300000000000002</v>
       </c>
-      <c r="K21">
+      <c r="J21" s="9">
+        <v>-3.95E-2</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
         <v>4.7300000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
@@ -907,11 +990,17 @@
       <c r="I22">
         <v>0.64600000000000002</v>
       </c>
-      <c r="K22">
+      <c r="J22" s="9">
+        <v>-2.2700000000000001E-2</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
         <v>8.6E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
@@ -936,11 +1025,17 @@
       <c r="I23">
         <v>0.66200000000000003</v>
       </c>
-      <c r="K23">
+      <c r="J23" s="9">
+        <v>-0.13289999999999999</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
@@ -965,11 +1060,17 @@
       <c r="I24">
         <v>0.57899999999999996</v>
       </c>
-      <c r="K24">
+      <c r="J24" s="9">
+        <v>-0.107</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -994,11 +1095,17 @@
       <c r="I25">
         <v>0.63400000000000001</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="9">
+        <v>-0.13469999999999999</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9">
         <v>3.2399999999999998E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1023,11 +1130,24 @@
       <c r="I26">
         <v>0.69399999999999995</v>
       </c>
-      <c r="K26">
+      <c r="J26" s="9">
+        <v>-6.3200000000000006E-2</v>
+      </c>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1052,20 +1172,23 @@
       <c r="I28" s="1">
         <v>0.82499999999999996</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="9">
+        <v>-6.9099999999999995E-2</v>
+      </c>
+      <c r="K28" s="10">
         <v>0.2641</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="10">
         <v>0.41620000000000001</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="10">
         <v>0.315</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="10">
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1090,20 +1213,23 @@
       <c r="I29" s="1">
         <v>0.70599999999999996</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="9">
+        <v>0.1847</v>
+      </c>
+      <c r="K29" s="10">
         <v>5.3800000000000001E-2</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="10">
         <v>0.13900000000000001</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="10">
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1128,24 +1254,30 @@
       <c r="I30" s="1">
         <v>0.79200000000000004</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="9">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="K30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L30" s="1">
+      <c r="M30" s="10">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="10">
         <v>0.2</v>
       </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>